<commit_message>
AO & ACS Interface
</commit_message>
<xml_diff>
--- a/Status/Importants(AutoRecovered).xlsx
+++ b/Status/Importants(AutoRecovered).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\opm\Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84E115F-3D0B-4541-AB2C-439EF2FEA2BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288A67D9-03BA-4B3E-B3C7-DCF3F9DB8133}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="1" xr2:uid="{EA588CC7-F7CD-441A-A2DF-E8EE0DE5ABCC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{EA588CC7-F7CD-441A-A2DF-E8EE0DE5ABCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -504,11 +510,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -533,18 +545,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1186,6 +1186,102 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2582334" y="5757333"/>
+          <a:ext cx="116417" cy="116417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>201084</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="116417" cy="116417"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Graphic 15" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC5B7853-F150-46B8-8C12-3544C052B641}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2582334" y="5947833"/>
+          <a:ext cx="116417" cy="116417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>201084</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="116417" cy="116417"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Graphic 16" descr="Checkmark">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05684F2F-5401-413B-A6F2-1F0640E0B39E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2582334" y="6138333"/>
           <a:ext cx="116417" cy="116417"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3255,8 +3351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81067F39-39BC-427C-B7A8-196E65E42EEC}">
   <dimension ref="A1:BF38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3266,177 +3362,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11" t="s">
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11" t="s">
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11" t="s">
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
-      <c r="AP1" s="11"/>
-      <c r="AQ1" s="11"/>
-      <c r="AR1" s="11"/>
-      <c r="AS1" s="11"/>
-      <c r="AT1" s="11"/>
-      <c r="AU1" s="11"/>
-      <c r="AV1" s="11"/>
-      <c r="AW1" s="11"/>
-      <c r="AX1" s="11"/>
-      <c r="AY1" s="11"/>
-      <c r="AZ1" s="11"/>
-      <c r="BA1" s="11"/>
-      <c r="BB1" s="11"/>
-      <c r="BC1" s="11"/>
-      <c r="BD1" s="11"/>
-      <c r="BE1" s="11"/>
-      <c r="BF1" s="11"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11" t="s">
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11" t="s">
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11" t="s">
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11" t="s">
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11" t="s">
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11" t="s">
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11" t="s">
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11" t="s">
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11" t="s">
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="11" t="s">
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11"/>
-      <c r="AU2" s="11" t="s">
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AV2" s="11"/>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="11" t="s">
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AY2" s="11"/>
-      <c r="AZ2" s="11"/>
-      <c r="BA2" s="11" t="s">
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="BB2" s="11"/>
-      <c r="BC2" s="11"/>
-      <c r="BD2" s="11" t="s">
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="BE2" s="11"/>
-      <c r="BF2" s="11"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12"/>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4480,10 +4576,10 @@
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4492,46 +4588,46 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>4</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>5</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="15"/>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19">
@@ -4659,23 +4755,25 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4683,7 +4781,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -4691,7 +4789,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -4699,7 +4797,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -4709,6 +4807,24 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="AX2:AZ2"/>
+    <mergeCell ref="BA2:BC2"/>
+    <mergeCell ref="BD2:BF2"/>
+    <mergeCell ref="AL1:BF1"/>
+    <mergeCell ref="AO2:AQ2"/>
+    <mergeCell ref="AR2:AT2"/>
+    <mergeCell ref="AC1:AK1"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="T1:AB1"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="E1:J1"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="K1:S1"/>
     <mergeCell ref="K2:M2"/>
@@ -4722,24 +4838,6 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="T1:AB1"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="AC1:AK1"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="AX2:AZ2"/>
-    <mergeCell ref="BA2:BC2"/>
-    <mergeCell ref="BD2:BF2"/>
-    <mergeCell ref="AL1:BF1"/>
-    <mergeCell ref="AO2:AQ2"/>
-    <mergeCell ref="AR2:AT2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4751,7 +4849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8FE945-70F7-4E8E-AF80-F13293216A78}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -5029,224 +5127,208 @@
   <sheetData>
     <row r="8" spans="9:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="9:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="AJ9" s="17" t="s">
+      <c r="J9" s="22"/>
+      <c r="AJ9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AK9" s="18"/>
-      <c r="AM9" s="17" t="s">
+      <c r="AK9" s="22"/>
+      <c r="AM9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="AN9" s="18"/>
-      <c r="AP9" s="17" t="s">
+      <c r="AN9" s="22"/>
+      <c r="AP9" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="AQ9" s="18"/>
-      <c r="AS9" s="17" t="s">
+      <c r="AQ9" s="22"/>
+      <c r="AS9" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AT9" s="18"/>
-      <c r="AV9" s="17" t="s">
+      <c r="AT9" s="22"/>
+      <c r="AV9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="AW9" s="18"/>
-      <c r="AY9" s="17" t="s">
+      <c r="AW9" s="22"/>
+      <c r="AY9" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AZ9" s="18"/>
-      <c r="BB9" s="17" t="s">
+      <c r="AZ9" s="22"/>
+      <c r="BB9" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="BC9" s="18"/>
+      <c r="BC9" s="22"/>
     </row>
     <row r="10" spans="9:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
-      <c r="AJ10" s="19"/>
-      <c r="AK10" s="20"/>
-      <c r="AM10" s="19"/>
-      <c r="AN10" s="20"/>
-      <c r="AP10" s="19"/>
-      <c r="AQ10" s="20"/>
-      <c r="AS10" s="19"/>
-      <c r="AT10" s="20"/>
-      <c r="AV10" s="19"/>
-      <c r="AW10" s="20"/>
-      <c r="AY10" s="19"/>
-      <c r="AZ10" s="20"/>
-      <c r="BB10" s="19"/>
-      <c r="BC10" s="20"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="24"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="24"/>
+      <c r="AP10" s="23"/>
+      <c r="AQ10" s="24"/>
+      <c r="AS10" s="23"/>
+      <c r="AT10" s="24"/>
+      <c r="AV10" s="23"/>
+      <c r="AW10" s="24"/>
+      <c r="AY10" s="23"/>
+      <c r="AZ10" s="24"/>
+      <c r="BB10" s="23"/>
+      <c r="BC10" s="24"/>
     </row>
     <row r="12" spans="9:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="9:55" x14ac:dyDescent="0.25">
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="AD13" s="17" t="s">
+      <c r="J13" s="22"/>
+      <c r="AD13" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AE13" s="18"/>
-      <c r="AG13" s="17" t="s">
+      <c r="AE13" s="22"/>
+      <c r="AG13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AH13" s="18"/>
+      <c r="AH13" s="22"/>
     </row>
     <row r="14" spans="9:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-      <c r="AD14" s="19"/>
-      <c r="AE14" s="20"/>
-      <c r="AG14" s="19"/>
-      <c r="AH14" s="20"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="24"/>
+      <c r="AG14" s="23"/>
+      <c r="AH14" s="24"/>
     </row>
     <row r="16" spans="9:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="X17" s="17" t="s">
+      <c r="J17" s="22"/>
+      <c r="X17" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="Y17" s="18"/>
-      <c r="AA17" s="17" t="s">
+      <c r="Y17" s="22"/>
+      <c r="AA17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="AB17" s="18"/>
-      <c r="AD17" s="17" t="s">
+      <c r="AB17" s="22"/>
+      <c r="AD17" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="AE17" s="18"/>
+      <c r="AE17" s="22"/>
     </row>
     <row r="18" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="20"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="20"/>
-      <c r="AD18" s="19"/>
-      <c r="AE18" s="20"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="24"/>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="24"/>
+      <c r="AD18" s="23"/>
+      <c r="AE18" s="24"/>
     </row>
     <row r="19" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="F20" s="25" t="s">
+      <c r="C20" s="18"/>
+      <c r="F20" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="26"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="18"/>
-      <c r="R22" s="21" t="s">
+      <c r="J22" s="22"/>
+      <c r="R22" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="S22" s="22"/>
-      <c r="U22" s="25" t="s">
+      <c r="S22" s="26"/>
+      <c r="U22" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="V22" s="26"/>
-      <c r="X22" s="21" t="s">
+      <c r="V22" s="18"/>
+      <c r="X22" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="Y22" s="22"/>
+      <c r="Y22" s="26"/>
     </row>
     <row r="23" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I23" s="19"/>
-      <c r="J23" s="20"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="24"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="28"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="24"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="28"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="20"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="28"/>
     </row>
     <row r="25" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="J26" s="18"/>
-      <c r="L26" s="25" t="s">
+      <c r="J26" s="22"/>
+      <c r="L26" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="26"/>
-      <c r="O26" s="25" t="s">
+      <c r="M26" s="18"/>
+      <c r="O26" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="P26" s="26"/>
-      <c r="R26" s="25" t="s">
+      <c r="P26" s="18"/>
+      <c r="R26" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="S26" s="26"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="19"/>
-      <c r="J27" s="20"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="28"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="28"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="28"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="24"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="20"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="20"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="20"/>
     </row>
     <row r="29" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="I30" s="17" t="s">
+      <c r="I30" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="J30" s="18"/>
-      <c r="L30" s="25" t="s">
+      <c r="J30" s="22"/>
+      <c r="L30" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="M30" s="26"/>
-      <c r="O30" s="25" t="s">
+      <c r="M30" s="18"/>
+      <c r="O30" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="P30" s="26"/>
+      <c r="P30" s="18"/>
     </row>
     <row r="31" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="28"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="28"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="24"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="20"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="I17:J18"/>
-    <mergeCell ref="X22:Y23"/>
-    <mergeCell ref="I26:J27"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L26:M27"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="I22:J23"/>
-    <mergeCell ref="O26:P27"/>
-    <mergeCell ref="O30:P31"/>
-    <mergeCell ref="R26:S27"/>
-    <mergeCell ref="R22:S23"/>
-    <mergeCell ref="U22:V23"/>
     <mergeCell ref="BB9:BC10"/>
     <mergeCell ref="X17:Y18"/>
     <mergeCell ref="AA17:AB18"/>
@@ -5259,6 +5341,22 @@
     <mergeCell ref="AS9:AT10"/>
     <mergeCell ref="AV9:AW10"/>
     <mergeCell ref="AY9:AZ10"/>
+    <mergeCell ref="X22:Y23"/>
+    <mergeCell ref="I26:J27"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L26:M27"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="I22:J23"/>
+    <mergeCell ref="O26:P27"/>
+    <mergeCell ref="O30:P31"/>
+    <mergeCell ref="R26:S27"/>
+    <mergeCell ref="R22:S23"/>
+    <mergeCell ref="U22:V23"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="I17:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>